<commit_message>
Changed the structure. Changes are made directly with querries to the DB. All classes were removed. Now 2 classes exist, one ofr connection and one to handle the querries
</commit_message>
<xml_diff>
--- a/My_Assets.xlsx
+++ b/My_Assets.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://openuniv-my.sharepoint.com/personal/rb26422_ou_ac_uk/Documents/Documents/OPEN UNIVERSITY/My PyCharm Projects/Data_Handling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - The Open University\Documents\OPEN UNIVERSITY\My PyCharm Projects\Data_Handling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="265" documentId="13_ncr:1_{6B62374D-B976-448F-B31C-43C5FE48FCA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93300F1F-B887-4A54-8741-88B2A028E634}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2278D20F-8C22-4A0A-9274-C8F1CF0D0CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{AB4DD51B-2067-4D03-B551-62E9035F195A}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
   <si>
     <t>QQQ</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>Crypto Asset</t>
+  </si>
+  <si>
+    <t>asset_ID</t>
   </si>
 </sst>
 </file>
@@ -222,10 +225,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -545,325 +544,328 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8795EA8D-A110-434C-9151-7A21DE58C361}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.19921875" customWidth="1"/>
-    <col min="2" max="2" width="17.59765625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.9296875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31.1328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.19921875" customWidth="1"/>
+    <col min="3" max="3" width="17.59765625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.9296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31.1328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C2" s="1">
         <v>1685</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="1" t="s">
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C3" s="1">
         <v>950</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="1">
+      <c r="C4" s="1">
         <v>810</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="1" t="s">
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="1">
+      <c r="C5" s="1">
         <v>770</v>
       </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="1" t="s">
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="1">
+      <c r="C6" s="1">
         <v>690</v>
       </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="1" t="s">
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="1">
+      <c r="C7" s="1">
         <v>600</v>
       </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" s="1" t="s">
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="1">
+      <c r="C8" s="1">
         <v>600</v>
       </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" s="1" t="s">
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="1">
+      <c r="C9" s="1">
         <v>570</v>
       </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" s="1" t="s">
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="1">
+      <c r="C10" s="1">
         <v>534</v>
       </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" s="1" t="s">
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="1">
+      <c r="C11" s="1">
         <v>490</v>
       </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12" s="1" t="s">
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="1">
+      <c r="C12" s="1">
         <v>441</v>
       </c>
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13" s="1" t="s">
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="1">
+      <c r="C13" s="1">
         <v>980</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="1">
+      <c r="C14" s="1">
         <v>610</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="1">
+      <c r="C15" s="1">
         <v>250</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="1">
+      <c r="C16" s="1">
         <v>1050</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="1">
+      <c r="C17" s="1">
         <v>770</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="1">
+      <c r="C18" s="1">
         <v>680</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="1">
+      <c r="C19" s="1">
         <v>495</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="1">
+      <c r="C20" s="1">
         <v>180</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="1">
+      <c r="C21" s="1">
         <v>1300</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="1">
+      <c r="C22" s="1">
         <v>625</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="1">
+      <c r="C23" s="1">
         <v>560</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="1">
+      <c r="C24" s="1">
         <v>500</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B25" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="1">
+      <c r="C25" s="1">
         <v>500</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B26" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="1">
+      <c r="C26" s="1">
         <v>480</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B27" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="1">
+      <c r="C27" s="1">
         <v>350</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B28" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="1">
+      <c r="C28" s="1">
         <v>208</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>